<commit_message>
Breytingar á losunar útreikningum og töflu
</commit_message>
<xml_diff>
--- a/heimildir.xlsx
+++ b/heimildir.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Svið\3. Orka\3.1. Orkumálaráðgjöf\Verkefnaoflun\Áburðarmál\aburdur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2348043D-6F8E-4B02-9819-3347E33723A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90B63C2-FEF8-4453-88EE-F4E9B99D967F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="17640" xr2:uid="{61A65F08-5524-4945-817E-387BD8820227}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{61A65F08-5524-4945-817E-387BD8820227}"/>
   </bookViews>
   <sheets>
     <sheet name="aburðartegundir" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
   <si>
     <t>Tegund áburðar</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>afylling_min</t>
+  </si>
+  <si>
+    <t>los_n</t>
   </si>
 </sst>
 </file>
@@ -594,15 +597,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43C59B6A-6CC9-4E6B-AA92-F8453F249335}">
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4:U5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -672,8 +680,11 @@
       <c r="W1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -734,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="U2">
-        <v>0.95</v>
+        <v>1.05</v>
       </c>
       <c r="V2">
         <f>losun!D3</f>
@@ -744,8 +755,12 @@
         <f>losun!E3</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X2">
+        <f>H2/100*(44/28)*0.01*298</f>
+        <v>1.1707142857142858</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -825,8 +840,12 @@
         <f>losun!E4</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3">
+        <f t="shared" ref="X3:X16" si="0">H3/100*(44/28)*0.01*298</f>
+        <v>4.3550571428571432E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -896,7 +915,7 @@
         <v>940</v>
       </c>
       <c r="U4">
-        <v>0.19</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="V4">
         <f>losun!D5</f>
@@ -906,8 +925,12 @@
         <f>losun!E5</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4">
+        <f t="shared" si="0"/>
+        <v>1.5921714285714286E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -971,7 +994,7 @@
         <v>940</v>
       </c>
       <c r="U5">
-        <v>0.19</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="V5">
         <f>losun!D6</f>
@@ -981,8 +1004,12 @@
         <f>losun!E6</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5">
+        <f t="shared" si="0"/>
+        <v>9.3657142857142869E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1063,8 +1090,12 @@
         <f>losun!E7</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X6">
+        <f t="shared" si="0"/>
+        <v>3.7462857142857145E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1145,8 +1176,12 @@
         <f>losun!E8</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X7">
+        <f t="shared" si="0"/>
+        <v>1.8263142857142856E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1227,8 +1262,12 @@
         <f>losun!E9</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8">
+        <f t="shared" si="0"/>
+        <v>8.8974285714285714E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1309,8 +1348,12 @@
         <f>losun!E10</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X9">
+        <f t="shared" si="0"/>
+        <v>0.13346142857142859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1380,7 +1423,7 @@
         <v>940</v>
       </c>
       <c r="U10">
-        <v>0.19</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="V10">
         <f>losun!D11</f>
@@ -1390,8 +1433,12 @@
         <f>losun!E11</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X10">
+        <f t="shared" si="0"/>
+        <v>0.4181791428571428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1472,8 +1519,12 @@
         <f>losun!E12</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X11">
+        <f t="shared" si="0"/>
+        <v>3.0438571428571436E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1553,8 +1604,12 @@
         <f>losun!E13</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X12">
+        <f t="shared" si="0"/>
+        <v>0.10302285714285715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1635,8 +1690,12 @@
         <f>losun!E14</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X13">
+        <f t="shared" si="0"/>
+        <v>6.2750285714285717E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1716,8 +1775,12 @@
         <f>losun!E15</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X14">
+        <f t="shared" si="0"/>
+        <v>3.5589714285714287E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1791,8 +1854,12 @@
         <f>losun!E16</f>
         <v>10.88</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X15">
+        <f t="shared" si="0"/>
+        <v>7.9608571428571445E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1872,6 +1939,10 @@
       <c r="W16">
         <f>losun!E17</f>
         <v>10.88</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="0"/>
+        <v>1.8263142857142856E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2073,7 +2144,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E17"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Forsendu breytingar - niturinnihald
</commit_message>
<xml_diff>
--- a/heimildir.xlsx
+++ b/heimildir.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Svið\3. Orka\3.1. Orkumálaráðgjöf\Verkefnaoflun\Áburðarmál\aburdur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhi\OneDrive - EFLA hf., verkfræðistofa\Documents\aburdur2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90B63C2-FEF8-4453-88EE-F4E9B99D967F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1D60F2-869D-45E0-B2BF-0C9064114FDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{61A65F08-5524-4945-817E-387BD8820227}"/>
+    <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="17640" xr2:uid="{61A65F08-5524-4945-817E-387BD8820227}"/>
   </bookViews>
   <sheets>
     <sheet name="aburðartegundir" sheetId="1" r:id="rId1"/>
@@ -601,7 +601,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U3" sqref="U3"/>
+      <selection pane="topRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +868,7 @@
         <v>200</v>
       </c>
       <c r="H4">
-        <v>0.34</v>
+        <v>0.45</v>
       </c>
       <c r="I4">
         <v>0.3</v>
@@ -927,7 +927,7 @@
       </c>
       <c r="X4">
         <f t="shared" si="0"/>
-        <v>1.5921714285714286E-2</v>
+        <v>2.1072857142857147E-2</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
         <v>200</v>
       </c>
       <c r="H8">
-        <v>1.9</v>
+        <v>2.76</v>
       </c>
       <c r="I8">
         <v>0.4</v>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>8.8974285714285714E-2</v>
+        <v>0.12924685714285714</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
         <v>200</v>
       </c>
       <c r="H9">
-        <v>2.85</v>
+        <v>3.58</v>
       </c>
       <c r="I9">
         <v>0.51</v>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>0.13346142857142859</v>
+        <v>0.16764628571428572</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1376,7 +1376,7 @@
         <v>100</v>
       </c>
       <c r="H10">
-        <v>8.93</v>
+        <v>9.35</v>
       </c>
       <c r="I10">
         <v>3.62</v>
@@ -1435,7 +1435,7 @@
       </c>
       <c r="X10">
         <f t="shared" si="0"/>
-        <v>0.4181791428571428</v>
+        <v>0.43784714285714288</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1461,7 +1461,7 @@
         <v>200</v>
       </c>
       <c r="H11">
-        <v>0.65</v>
+        <v>0.27</v>
       </c>
       <c r="I11">
         <v>0.09</v>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="X11">
         <f t="shared" si="0"/>
-        <v>3.0438571428571436E-2</v>
+        <v>1.2643714285714286E-2</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1547,7 +1547,7 @@
         <v>200</v>
       </c>
       <c r="H12">
-        <v>2.2000000000000002</v>
+        <v>1.31</v>
       </c>
       <c r="I12">
         <v>0.26</v>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="X12">
         <f t="shared" si="0"/>
-        <v>0.10302285714285715</v>
+        <v>6.1345428571428579E-2</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1718,7 +1718,7 @@
         <v>200</v>
       </c>
       <c r="H14">
-        <v>0.76</v>
+        <v>0.88</v>
       </c>
       <c r="I14">
         <v>0.09</v>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="X14">
         <f t="shared" si="0"/>
-        <v>3.5589714285714287E-2</v>
+        <v>4.1209142857142861E-2</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Breyting á dreifingu kjötmjöls
</commit_message>
<xml_diff>
--- a/heimildir.xlsx
+++ b/heimildir.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhi\OneDrive - EFLA hf., verkfræðistofa\Documents\aburdur2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Svið\3. Orka\3.1. Orkumálaráðgjöf\Verkefnaoflun\Áburðarmál\aburdur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1D60F2-869D-45E0-B2BF-0C9064114FDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8928FCF-DDCE-4B9A-83B9-4C3722725633}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-285" windowWidth="29040" windowHeight="17640" xr2:uid="{61A65F08-5524-4945-817E-387BD8820227}"/>
   </bookViews>
@@ -601,7 +601,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H15" sqref="H15"/>
+      <selection pane="topRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,7 +1373,7 @@
         <v>20</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H10">
         <v>9.35</v>

</xml_diff>